<commit_message>
Se agrega indicador de Dato obligatoro en los formularios de creacion de registros de Inventarios
</commit_message>
<xml_diff>
--- a/public/DownloadExcels/Materias_Primas.xlsx
+++ b/public/DownloadExcels/Materias_Primas.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Mario\Desktop\Ecopcion Desarrollo\ecopFront-Desarrollo\public\DownloadExcels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B972856-956A-46CF-A751-832C0835E4C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B217CA6C-3066-4A1A-AA37-BEAAA523EF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INVENTARIO DE MATERIAS PRIMAS" sheetId="1" r:id="rId1"/>
-    <sheet name="Lista desplegable" sheetId="2" r:id="rId2"/>
+    <sheet name="INSTRUCCIONES" sheetId="3" r:id="rId2"/>
+    <sheet name="Lista desplegable" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
   <si>
     <t>INVENTARIO DE MATERIAS PRIMAS / INSUMOS</t>
   </si>
@@ -357,6 +358,9 @@
   </si>
   <si>
     <t>Frasco</t>
+  </si>
+  <si>
+    <t>Botella</t>
   </si>
 </sst>
 </file>
@@ -805,6 +809,12 @@
     <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -819,12 +829,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1095,7 +1099,7 @@
   <dimension ref="A1:AA899"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1111,61 +1115,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
     </row>
     <row r="2" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
     </row>
     <row r="3" spans="1:27" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="65"/>
     </row>
     <row r="4" spans="1:27" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17"/>
@@ -16944,7 +16948,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{95CA0C82-AAD2-46BE-9368-E5A4E9443D01}">
           <x14:formula1>
-            <xm:f>'Lista desplegable'!$B$2:$B$31</xm:f>
+            <xm:f>'Lista desplegable'!$B$2:$B$32</xm:f>
           </x14:formula1>
           <xm:sqref>E6:E205</xm:sqref>
         </x14:dataValidation>
@@ -16955,11 +16959,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F778330C-B888-4E1F-9D51-6576E83C0DAD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:J999"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17171,7 +17187,7 @@
       </c>
     </row>
     <row r="9" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="59" t="s">
         <v>4</v>
       </c>
       <c r="F9" s="28">
@@ -17185,7 +17201,7 @@
       </c>
     </row>
     <row r="10" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="60" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="28">
@@ -17207,8 +17223,8 @@
       </c>
     </row>
     <row r="12" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="65" t="s">
-        <v>14</v>
+      <c r="B12" s="27" t="s">
+        <v>67</v>
       </c>
       <c r="F12" s="28">
         <v>6</v>
@@ -17216,8 +17232,8 @@
       <c r="G12" s="50"/>
     </row>
     <row r="13" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="27" t="s">
-        <v>65</v>
+      <c r="B13" s="60" t="s">
+        <v>14</v>
       </c>
       <c r="F13" s="28">
         <v>7</v>
@@ -17225,139 +17241,141 @@
     </row>
     <row r="14" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F14" s="28">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="65" t="s">
-        <v>15</v>
+      <c r="B15" s="27" t="s">
+        <v>66</v>
       </c>
       <c r="F15" s="28">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="65" t="s">
-        <v>16</v>
+      <c r="B16" s="60" t="s">
+        <v>15</v>
       </c>
       <c r="F16" s="28">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="65" t="s">
-        <v>17</v>
+      <c r="B17" s="60" t="s">
+        <v>16</v>
       </c>
       <c r="F17" s="28">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="65" t="s">
-        <v>18</v>
+      <c r="B18" s="60" t="s">
+        <v>17</v>
       </c>
       <c r="F18" s="28">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="65" t="s">
-        <v>19</v>
+      <c r="B19" s="60" t="s">
+        <v>18</v>
       </c>
       <c r="F19" s="28">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="65" t="s">
-        <v>20</v>
+      <c r="B20" s="60" t="s">
+        <v>19</v>
       </c>
       <c r="F20" s="28">
         <v>35</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="65" t="s">
-        <v>21</v>
+      <c r="B21" s="60" t="s">
+        <v>20</v>
       </c>
       <c r="G21" s="50"/>
       <c r="H21" s="53"/>
     </row>
     <row r="22" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="65" t="s">
-        <v>22</v>
+      <c r="B22" s="60" t="s">
+        <v>21</v>
       </c>
       <c r="G22" s="50"/>
       <c r="H22" s="53"/>
     </row>
     <row r="23" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="9" t="s">
-        <v>23</v>
+      <c r="B23" s="60" t="s">
+        <v>22</v>
       </c>
       <c r="G23" s="50"/>
       <c r="H23" s="53"/>
     </row>
     <row r="24" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G24" s="50"/>
       <c r="H24" s="53"/>
     </row>
     <row r="25" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G25" s="50"/>
       <c r="H25" s="53"/>
     </row>
     <row r="26" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G26" s="50"/>
       <c r="H26" s="53"/>
     </row>
     <row r="27" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G27" s="50"/>
       <c r="H27" s="53"/>
     </row>
     <row r="28" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G28" s="50"/>
       <c r="H28" s="53"/>
     </row>
     <row r="29" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G29" s="50"/>
       <c r="H29" s="53"/>
     </row>
     <row r="30" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G30" s="50"/>
       <c r="H30" s="53"/>
     </row>
     <row r="31" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G31" s="50"/>
       <c r="H31" s="53"/>
     </row>
     <row r="32" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
+      <c r="B32" s="9" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="33" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>

</xml_diff>